<commit_message>
updated Tao excel document with observation notes
</commit_message>
<xml_diff>
--- a/Tao_Enrichment_080621_github.xlsx
+++ b/Tao_Enrichment_080621_github.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tao1/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stanford/ENCODE_K562/github/K562-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CF8075-FA20-0D4A-A33F-79610F2E2E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECDBEBF-AD3B-0A4F-898B-EADA4C05A3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16240" activeTab="2" xr2:uid="{56FA5575-6236-5941-B9FF-001EC709D4B0}"/>
+    <workbookView xWindow="9060" yWindow="460" windowWidth="25040" windowHeight="16240" xr2:uid="{56FA5575-6236-5941-B9FF-001EC709D4B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="344">
   <si>
     <t>Cluster_ID</t>
   </si>
@@ -1044,6 +1044,30 @@
   </si>
   <si>
     <t>https://www.vierstra.org/resources/dgf</t>
+  </si>
+  <si>
+    <t>TF Signal at peaks with SNPs</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>left skew</t>
+  </si>
+  <si>
+    <t>right skew</t>
+  </si>
+  <si>
+    <t>Uniform</t>
+  </si>
+  <si>
+    <t>Motif Effect (Mismatch/Match)</t>
+  </si>
+  <si>
+    <t>Bimodal</t>
+  </si>
+  <si>
+    <t>SNP Position</t>
   </si>
 </sst>
 </file>
@@ -1485,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E2CB9E-72B5-2046-BF2C-61181C6331BB}">
-  <dimension ref="A1:L134"/>
+  <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,10 +1525,12 @@
     <col min="9" max="9" width="28.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,6 +1555,9 @@
       <c r="H1" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>336</v>
+      </c>
       <c r="J1" s="2" t="s">
         <v>272</v>
       </c>
@@ -1538,8 +1567,14 @@
       <c r="L1" s="2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>106</v>
       </c>
@@ -1576,8 +1611,14 @@
       <c r="L2" s="7" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>337</v>
+      </c>
+      <c r="N2">
+        <v>7.4268999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>121</v>
       </c>
@@ -1615,8 +1656,14 @@
       <c r="L3" s="7" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>338</v>
+      </c>
+      <c r="N3">
+        <v>36.555599999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>113</v>
       </c>
@@ -1653,8 +1700,14 @@
       <c r="L4" s="7" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>337</v>
+      </c>
+      <c r="N4">
+        <v>1.8684000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>113</v>
       </c>
@@ -1691,8 +1744,14 @@
       <c r="L5" s="7" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>342</v>
+      </c>
+      <c r="N5">
+        <v>1.5784899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>109</v>
       </c>
@@ -1730,8 +1789,14 @@
       <c r="L6" s="7" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>337</v>
+      </c>
+      <c r="N6">
+        <v>1.7824800000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>109</v>
       </c>
@@ -1769,8 +1834,14 @@
       <c r="L7" s="7" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>340</v>
+      </c>
+      <c r="N7">
+        <v>1.6472800000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>109</v>
       </c>
@@ -1808,8 +1879,14 @@
       <c r="L8" s="7" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>339</v>
+      </c>
+      <c r="N8">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>109</v>
       </c>
@@ -1847,8 +1924,14 @@
       <c r="L9" s="7" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>337</v>
+      </c>
+      <c r="N9">
+        <v>1.7809699999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>109</v>
       </c>
@@ -1886,8 +1969,14 @@
       <c r="L10" s="7" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>339</v>
+      </c>
+      <c r="N10">
+        <v>2.4161700000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>109</v>
       </c>
@@ -1925,8 +2014,14 @@
       <c r="L11" s="7" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>340</v>
+      </c>
+      <c r="N11">
+        <v>1.93638</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>109</v>
       </c>
@@ -1964,8 +2059,14 @@
       <c r="L12" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>340</v>
+      </c>
+      <c r="N12">
+        <v>2.04623</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>73</v>
       </c>
@@ -2003,8 +2104,14 @@
       <c r="L13" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>340</v>
+      </c>
+      <c r="N13">
+        <v>31.8627</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>115</v>
       </c>
@@ -2042,8 +2149,14 @@
       <c r="L14" s="7" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>340</v>
+      </c>
+      <c r="N14">
+        <v>26.230799999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>106</v>
       </c>
@@ -2059,7 +2172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>106</v>
       </c>
@@ -4066,6 +4179,16 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H134">
     <sortCondition ref="G2:G134"/>
   </sortState>
+  <conditionalFormatting sqref="N2:N14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" tooltip="Go to page for ENCFF847HGM" display="https://www.encodeproject.org/files/ENCFF847HGM/" xr:uid="{9603BE6C-DD6F-1040-9A3E-DFC17B1E3E0F}"/>
     <hyperlink ref="L2" r:id="rId2" tooltip="Go to page for ENCFF557FUM" display="https://www.encodeproject.org/files/ENCFF557FUM/" xr:uid="{011D440D-08C5-F745-AA98-259AB596BD6E}"/>
@@ -4664,7 +4787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9AD2361-A8A1-C04C-91B2-973D313E7F3B}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>